<commit_message>
Cambios en una materia y organización en horas de estudio
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\OneDrive\Documents\Udea\Info 2\Teoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB1C45C6-ACC3-43EF-87A5-6BF0BDE7C14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488A48A0-F93E-40BD-90EA-549A0FCF6854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2EF7DFA1-8FCD-4007-86E5-010A26321E6F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="36">
   <si>
     <t>Lab. Señales</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Viernes 10</t>
+  </si>
+  <si>
+    <t>Repaso señales</t>
+  </si>
+  <si>
+    <t>Repaso estado solido</t>
+  </si>
+  <si>
+    <t>Estudiar estado solido</t>
+  </si>
+  <si>
+    <t>Practica lab info 2</t>
   </si>
 </sst>
 </file>
@@ -529,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C222B0-29C0-4AB5-82D8-4B38875486AA}">
   <dimension ref="B1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,9 +767,13 @@
       <c r="N4" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="O4" s="4"/>
+      <c r="O4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
+      <c r="Q4" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="R4" s="4"/>
       <c r="S4" s="4" t="s">
         <v>9</v>
@@ -765,9 +781,13 @@
       <c r="T4" s="2">
         <v>0.41666666666666669</v>
       </c>
-      <c r="U4" s="4"/>
+      <c r="U4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
+      <c r="W4" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="4" t="s">
         <v>9</v>
@@ -805,9 +825,13 @@
       <c r="N5" s="2">
         <v>0.45833333333333298</v>
       </c>
-      <c r="O5" s="4"/>
+      <c r="O5" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4" t="s">
         <v>9</v>
@@ -815,9 +839,13 @@
       <c r="T5" s="2">
         <v>0.45833333333333298</v>
       </c>
-      <c r="U5" s="4"/>
+      <c r="U5" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
+      <c r="W5" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="X5" s="4"/>
       <c r="Y5" s="4" t="s">
         <v>9</v>
@@ -1216,223 +1244,247 @@
         <v>0.75</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H12" s="2">
         <v>0.75</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M12" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="N12" s="2">
         <v>0.75</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="R12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S12" s="4"/>
+      <c r="S12" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="T12" s="2">
         <v>0.75</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="V12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="W12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="X12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y12" s="4"/>
+      <c r="Y12" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>0.79166666666666696</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H13" s="2">
         <v>0.79166666666666696</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J13" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M13" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="N13" s="2">
         <v>0.79166666666666696</v>
       </c>
-      <c r="O13" s="4"/>
+      <c r="O13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="P13" s="4" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="Q13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S13" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="T13" s="2">
         <v>0.79166666666666696</v>
       </c>
-      <c r="U13" s="4"/>
+      <c r="U13" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="V13" s="4" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="W13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y13" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="Y13" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>0.83333333333333304</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="D14" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H14" s="2">
         <v>0.83333333333333304</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="J14" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="M14" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="N14" s="2">
         <v>0.83333333333333304</v>
       </c>
-      <c r="O14" s="4"/>
+      <c r="O14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="P14" s="4" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="Q14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="S14" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="T14" s="2">
         <v>0.83333333333333304</v>
       </c>
-      <c r="U14" s="4"/>
+      <c r="U14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="V14" s="4" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="W14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y14" s="4"/>
+        <v>35</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>0.875</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="2">
         <v>0.875</v>
       </c>
-      <c r="I15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="M15" s="4"/>
       <c r="N15" s="2">
         <v>0.875</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="R15" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="S15" s="4"/>
       <c r="T15" s="2">
         <v>0.875</v>
       </c>
-      <c r="U15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V15" s="4"/>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
+      <c r="X15" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
@@ -1443,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="2">
@@ -1459,13 +1511,11 @@
         <v>6</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="2">
@@ -1475,13 +1525,13 @@
         <v>6</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="S16" s="4"/>
       <c r="T16" s="2">
@@ -1491,13 +1541,13 @@
         <v>6</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="Y16" s="4"/>
     </row>
@@ -1531,7 +1581,9 @@
       </c>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
+      <c r="W17" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
     </row>

</xml_diff>

<commit_message>
Modificacion del horario luego de pasado las semanas
</commit_message>
<xml_diff>
--- a/Calendario.xlsx
+++ b/Calendario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\OneDrive\Documents\Udea\Info 2\Teoria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488A48A0-F93E-40BD-90EA-549A0FCF6854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2884EC-5C34-4D3D-B801-5C0A94803299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2EF7DFA1-8FCD-4007-86E5-010A26321E6F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="36">
   <si>
     <t>Lab. Señales</t>
   </si>
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C222B0-29C0-4AB5-82D8-4B38875486AA}">
   <dimension ref="B1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,9 +902,7 @@
         <v>4</v>
       </c>
       <c r="W6" s="4"/>
-      <c r="X6" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="X6" s="4"/>
       <c r="Y6" s="4" t="s">
         <v>9</v>
       </c>
@@ -954,9 +952,7 @@
         <v>4</v>
       </c>
       <c r="W7" s="4"/>
-      <c r="X7" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="2:25" x14ac:dyDescent="0.25">
@@ -1026,9 +1022,7 @@
       <c r="W8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="X8" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="X8" s="4"/>
       <c r="Y8" s="4" t="s">
         <v>1</v>
       </c>
@@ -1143,9 +1137,7 @@
       <c r="R10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="S10" s="4"/>
       <c r="T10" s="2">
         <v>0.66666666666666696</v>
       </c>
@@ -1217,9 +1209,7 @@
       <c r="R11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="S11" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="S11" s="4"/>
       <c r="T11" s="2">
         <v>0.70833333333333304</v>
       </c>
@@ -1283,9 +1273,7 @@
       <c r="W12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Y12" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
@@ -1357,9 +1345,7 @@
       <c r="X13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Y13" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
@@ -1431,9 +1417,7 @@
       <c r="X14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Y14" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
@@ -1478,9 +1462,7 @@
         <v>0.875</v>
       </c>
       <c r="U15" s="4"/>
-      <c r="V15" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4" t="s">
         <v>35</v>
@@ -1546,9 +1528,7 @@
       <c r="W16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="X16" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
     </row>
     <row r="17" spans="2:25" x14ac:dyDescent="0.25">

</xml_diff>